<commit_message>
Update Test Data Excel Template
Add some more options (loop, pid increase, ...)
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/FHIR_Testdatengenerator_Vorlage.xlsx
+++ b/src/main/resources/excel/FHIR_Testdatengenerator_Vorlage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\TestDataGenerator\input - Vorlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2D7EFC-FBCA-42BB-8D5C-32978C2AB3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF101159-0E7C-4524-ABBD-CAF01F1ADC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="828" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="828" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="2" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="1045">
   <si>
     <t>Patient-ID</t>
   </si>
@@ -2927,42 +2927,12 @@
     <t>Zeitstempel = Datum und Urzeit der Messung</t>
   </si>
   <si>
-    <t>#####################################</t>
-  </si>
-  <si>
-    <t># Options to control the conversion #</t>
-  </si>
-  <si>
     <t>###</t>
   </si>
   <si>
     <t># Start index counter for the number that will be</t>
   </si>
   <si>
-    <t># START_ID_CONSENT = 1</t>
-  </si>
-  <si>
-    <t># START_ID_DIAGNOSIS = 1</t>
-  </si>
-  <si>
-    <t># START_ID_ENCOUNTER_LEVEL_2 = 1</t>
-  </si>
-  <si>
-    <t># START_ID_MEDICATION_ADMINISTRATION = 1</t>
-  </si>
-  <si>
-    <t># START_ID_MEDICATION_STATEMENT = 1</t>
-  </si>
-  <si>
-    <t># START_ID_OBSERVATION_LABORATORY = 1</t>
-  </si>
-  <si>
-    <t># START_ID_OBSERVATION_VITAL_SIGNS = 1</t>
-  </si>
-  <si>
-    <t># START_ID_PROCEDURE = 1</t>
-  </si>
-  <si>
     <t># If true, then Sub Encounters will have a diagnosis</t>
   </si>
   <si>
@@ -3026,9 +2996,6 @@
     <t># If the value is missing or commented out in this</t>
   </si>
   <si>
-    <t># map then the  default is 1.</t>
-  </si>
-  <si>
     <t xml:space="preserve"># Enable to set a the optional reference from </t>
   </si>
   <si>
@@ -3159,6 +3126,111 @@
   </si>
   <si>
     <t>numerischer Wert der Messung (auch negativ), optional mit einem der 4 Vergleichsoperatoren &lt;, &lt;=,  &gt;= oder &gt; davor</t>
+  </si>
+  <si>
+    <t># The last number in all patient IDs of an data set will be increased</t>
+  </si>
+  <si>
+    <t># by this value. At the beginning this number will be added to all</t>
+  </si>
+  <si>
+    <t># patient IDs.</t>
+  </si>
+  <si>
+    <t># Default value is 0.</t>
+  </si>
+  <si>
+    <t># PID_LAST_NUMBER_INCREASE_INITIAL_OFFSET = 0</t>
+  </si>
+  <si>
+    <t># by this value on every loop. This number should be greater or equal</t>
+  </si>
+  <si>
+    <t># to the difference between the highest and the lowast number in all</t>
+  </si>
+  <si>
+    <t># patient IDs. If not then some patients can be generated with the same</t>
+  </si>
+  <si>
+    <t># ID.</t>
+  </si>
+  <si>
+    <t># PID_LAST_NUMBER_INCREASE_LOOP_OFFSET = 0</t>
+  </si>
+  <si>
+    <t># Count of repetitions of increasings of the patient ID. If you want to</t>
+  </si>
+  <si>
+    <t># expand a data set n times then set this value to n and the</t>
+  </si>
+  <si>
+    <t># PID_LAST_NUMBER_INCREASE_START_OFFSET in the described way.</t>
+  </si>
+  <si>
+    <t># PID_LAST_NUMBER_INCREASE_LOOP_COUNT = 0</t>
+  </si>
+  <si>
+    <t># map then the default is 1.</t>
+  </si>
+  <si>
+    <t>#START_ID_CONSENT = 1</t>
+  </si>
+  <si>
+    <t>#START_ID_DIAGNOSIS = 1</t>
+  </si>
+  <si>
+    <t>#START_ID_ENCOUNTER_LEVEL_2 = 1</t>
+  </si>
+  <si>
+    <t>#START_ID_MEDICATION_ADMINISTRATION = 1</t>
+  </si>
+  <si>
+    <t>#START_ID_MEDICATION_STATEMENT = 1</t>
+  </si>
+  <si>
+    <t>#START_ID_OBSERVATION_LABORATORY = 1</t>
+  </si>
+  <si>
+    <t>#START_ID_OBSERVATION_VITAL_SIGNS = 1</t>
+  </si>
+  <si>
+    <t>#START_ID_PROCEDURE = 1</t>
+  </si>
+  <si>
+    <t># This prefix will be added to all patient IDs.</t>
+  </si>
+  <si>
+    <t># The default is an empty string.</t>
+  </si>
+  <si>
+    <t># PID_PREFIX = ANY_STRING</t>
+  </si>
+  <si>
+    <t># This suffix will be added to all patient IDs.</t>
+  </si>
+  <si>
+    <t># PID_SUFFIX = ANY_STRING</t>
+  </si>
+  <si>
+    <t># set. Use multiple converter option sheets #</t>
+  </si>
+  <si>
+    <t># converter option files for the same data  #</t>
+  </si>
+  <si>
+    <t># There can be defined multiple of this     #</t>
+  </si>
+  <si>
+    <t># Options to control the conversion.        #</t>
+  </si>
+  <si>
+    <t>#############################################</t>
+  </si>
+  <si>
+    <t># to create resources with different        #</t>
+  </si>
+  <si>
+    <t># references to each other.                 #</t>
   </si>
 </sst>
 </file>
@@ -3376,7 +3448,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -3473,6 +3545,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Erklärender Text" xfId="4" builtinId="53"/>
@@ -4246,7 +4320,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="71" t="s">
-        <v>1010</v>
+        <v>999</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -7882,9 +7956,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961B0353-4A30-49CF-9E96-AB439FF3F972}">
-  <dimension ref="A1:A108"/>
+  <dimension ref="A1:A150"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -7894,464 +7970,462 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="74" t="s">
-        <v>943</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="74" t="s">
-        <v>944</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="74" t="s">
-        <v>943</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="74"/>
+      <c r="A4" s="74" t="s">
+        <v>1039</v>
+      </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="74" t="s">
-        <v>945</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="74" t="s">
-        <v>946</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="74" t="s">
-        <v>971</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="74" t="s">
-        <v>972</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="74" t="s">
-        <v>973</v>
-      </c>
+      <c r="A9" s="74"/>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="74" t="s">
-        <v>974</v>
+        <v>943</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="74" t="s">
-        <v>975</v>
+        <v>944</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="74" t="s">
-        <v>976</v>
+        <v>961</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="74" t="s">
-        <v>945</v>
+        <v>962</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="74" t="s">
-        <v>947</v>
+        <v>963</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="74" t="s">
-        <v>948</v>
+        <v>964</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="74" t="s">
-        <v>949</v>
+        <v>965</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="74" t="s">
-        <v>950</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="74" t="s">
-        <v>951</v>
+        <v>943</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="74" t="s">
-        <v>952</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="74" t="s">
-        <v>953</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="74" t="s">
-        <v>954</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="74"/>
+      <c r="A22" s="74" t="s">
+        <v>1028</v>
+      </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="74"/>
+      <c r="A23" s="74" t="s">
+        <v>1029</v>
+      </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="74" t="s">
-        <v>945</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="74" t="s">
-        <v>977</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="74" t="s">
-        <v>993</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="74" t="s">
-        <v>985</v>
-      </c>
+      <c r="A27" s="74"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="74" t="s">
-        <v>994</v>
-      </c>
+      <c r="A28" s="74"/>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="74" t="s">
-        <v>995</v>
+        <v>943</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="74" t="s">
-        <v>978</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="74" t="s">
-        <v>979</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="74" t="s">
-        <v>996</v>
+        <v>943</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="74" t="s">
-        <v>980</v>
+      <c r="A33" s="78" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="74" t="s">
-        <v>981</v>
-      </c>
+      <c r="A34" s="74"/>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="74" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="74" t="s">
-        <v>992</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="74" t="s">
-        <v>982</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="74"/>
+      <c r="A38" s="74" t="s">
+        <v>943</v>
+      </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="74" t="s">
-        <v>983</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="74" t="s">
-        <v>984</v>
-      </c>
+      <c r="A40" s="74"/>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="74" t="s">
-        <v>997</v>
+        <v>943</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="74" t="s">
-        <v>985</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="74" t="s">
-        <v>998</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="74" t="s">
-        <v>986</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="74" t="s">
-        <v>987</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="75" t="s">
-        <v>988</v>
+        <v>943</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="75" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="75" t="s">
-        <v>980</v>
+      <c r="A47" s="79" t="s">
+        <v>1014</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="75" t="s">
-        <v>989</v>
+        <v>943</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="75" t="s">
-        <v>945</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="75" t="s">
-        <v>1000</v>
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="75" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="75" t="s">
+        <v>1017</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="75" t="s">
-        <v>945</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="75" t="s">
-        <v>977</v>
+        <v>943</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="75" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="75" t="s">
-        <v>985</v>
+      <c r="A56" s="79" t="s">
+        <v>1019</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="75" t="s">
-        <v>994</v>
+        <v>943</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="75" t="s">
-        <v>1002</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="75" t="s">
-        <v>978</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="75" t="s">
-        <v>979</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="75" t="s">
-        <v>1003</v>
+        <v>943</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="75" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="75" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="75" t="s">
-        <v>945</v>
+      <c r="A63" s="79" t="s">
+        <v>1023</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="75" t="s">
-        <v>1004</v>
+        <v>943</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="75" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="75" t="s">
         <v>982</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="75" t="s">
-        <v>983</v>
+        <v>974</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="75" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="75" t="s">
-        <v>1005</v>
+        <v>984</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="75" t="s">
-        <v>985</v>
+        <v>967</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="75" t="s">
-        <v>1006</v>
+        <v>968</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="75" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="75" t="s">
-        <v>987</v>
+        <v>969</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="75" t="s">
-        <v>988</v>
+        <v>970</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="75" t="s">
-        <v>1007</v>
+        <v>943</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="75" t="s">
-        <v>980</v>
+      <c r="A78" s="79" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="75" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="75" t="s">
-        <v>945</v>
+        <v>971</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="75" t="s">
-        <v>1008</v>
+        <v>972</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="75" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="75" t="s">
+        <v>986</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="75" t="s">
-        <v>945</v>
+        <v>974</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="75" t="s">
-        <v>955</v>
+        <v>987</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="75" t="s">
-        <v>956</v>
+        <v>975</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="75" t="s">
-        <v>957</v>
+        <v>976</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="75" t="s">
-        <v>958</v>
+        <v>977</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="75" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="75" t="s">
-        <v>960</v>
+        <v>969</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="75" t="s">
-        <v>961</v>
+        <v>978</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="75" t="s">
-        <v>962</v>
+        <v>943</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="75" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="75" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" s="75" t="s">
-        <v>990</v>
+      <c r="A93" s="79" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="75" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="75" t="s">
+        <v>966</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="75" t="s">
-        <v>945</v>
+        <v>990</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="75" t="s">
-        <v>964</v>
+        <v>974</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="75" t="s">
-        <v>965</v>
+        <v>983</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="75" t="s">
-        <v>966</v>
+        <v>991</v>
       </c>
     </row>
     <row r="102" spans="1:1">
@@ -8366,27 +8440,212 @@
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="75" t="s">
-        <v>969</v>
+        <v>992</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="75" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="75" t="s">
-        <v>963</v>
+        <v>970</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="75" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="79" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="75" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="75" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="75" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="75" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="75" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="75" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="75" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="75" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="75" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="75" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="75" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="75" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="75" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="79" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="75" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="75" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
-      <c r="A108" s="75" t="s">
-        <v>991</v>
+    <row r="128" spans="1:1">
+      <c r="A128" s="75" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="75" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="75" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="75" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="75" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="75" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="75" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="75" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="75" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="79" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="75" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="75" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="75" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="75" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="75" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="75" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="75" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="75" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="75" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="75" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="79" t="s">
+        <v>980</v>
       </c>
     </row>
   </sheetData>
@@ -9743,7 +10002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I928"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -9963,10 +10222,10 @@
         <v>43553</v>
       </c>
       <c r="H8" s="71" t="s">
-        <v>1012</v>
+        <v>1001</v>
       </c>
       <c r="I8" s="71" t="s">
-        <v>1013</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -9992,10 +10251,10 @@
         <v>43554</v>
       </c>
       <c r="H9" s="71" t="s">
-        <v>1014</v>
+        <v>1003</v>
       </c>
       <c r="I9" s="71" t="s">
-        <v>1015</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -10021,10 +10280,10 @@
         <v>43555</v>
       </c>
       <c r="H10" s="71" t="s">
-        <v>1011</v>
+        <v>1000</v>
       </c>
       <c r="I10" s="71" t="s">
-        <v>1020</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -10050,10 +10309,10 @@
         <v>43556</v>
       </c>
       <c r="H11" s="71" t="s">
-        <v>1016</v>
+        <v>1005</v>
       </c>
       <c r="I11" s="71" t="s">
-        <v>1017</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -10079,10 +10338,10 @@
         <v>43557</v>
       </c>
       <c r="H12" s="71" t="s">
-        <v>1018</v>
+        <v>1007</v>
       </c>
       <c r="I12" s="71" t="s">
-        <v>1019</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -26853,7 +27112,7 @@
         <v>103</v>
       </c>
       <c r="E2" s="76" t="s">
-        <v>1009</v>
+        <v>998</v>
       </c>
       <c r="F2" s="76"/>
       <c r="G2" s="76"/>
@@ -29420,15 +29679,53 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="15b42a90-06dd-4669-ae82-892e5974bb2f">TMFEV-111023110-895</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="15b42a90-06dd-4669-ae82-892e5974bb2f">
-      <Url>https://tmfev.sharepoint.com/sites/tmf/mi-i/_layouts/15/DocIdRedir.aspx?ID=TMFEV-111023110-895</Url>
-      <Description>TMFEV-111023110-895</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29673,53 +29970,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="15b42a90-06dd-4669-ae82-892e5974bb2f">TMFEV-111023110-895</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="15b42a90-06dd-4669-ae82-892e5974bb2f">
+      <Url>https://tmfev.sharepoint.com/sites/tmf/mi-i/_layouts/15/DocIdRedir.aspx?ID=TMFEV-111023110-895</Url>
+      <Description>TMFEV-111023110-895</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29732,11 +29991,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B89C2DA-DD1E-4298-9623-BC864CA91962}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17381246-8561-41AA-90B8-1B77E21DFFC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="15b42a90-06dd-4669-ae82-892e5974bb2f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -29762,9 +30019,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17381246-8561-41AA-90B8-1B77E21DFFC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B89C2DA-DD1E-4298-9623-BC864CA91962}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="15b42a90-06dd-4669-ae82-892e5974bb2f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>